<commit_message>
updated SQLite and tag metadata for nicer examples
</commit_message>
<xml_diff>
--- a/inst/extdata/tags_watlas_subset.xlsx
+++ b/inst/extdata/tags_watlas_subset.xlsx
@@ -1,80 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28129"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkrietsch\GitHub_R_packages\tools4watlas\inst\extdata\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E66B410-B54E-4B07-9393-748DE3BA1535}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30705" yWindow="1905" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="tags_watlas_all" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
-  <si>
-    <t>season</t>
-  </si>
-  <si>
-    <t>species</t>
-  </si>
-  <si>
-    <t>tag</t>
-  </si>
-  <si>
-    <t>rings</t>
-  </si>
-  <si>
-    <t>crc</t>
-  </si>
-  <si>
-    <t>release_ts</t>
-  </si>
-  <si>
-    <t>catch_location</t>
-  </si>
-  <si>
-    <t>redshank</t>
-  </si>
-  <si>
-    <t>1598631</t>
-  </si>
-  <si>
-    <t>griend</t>
-  </si>
-  <si>
-    <t>red knot</t>
-  </si>
-  <si>
-    <t>Z108969</t>
-  </si>
-  <si>
-    <t>Y7PRRG</t>
-  </si>
-  <si>
-    <t>Z108971</t>
-  </si>
-  <si>
-    <t>Y7PRRN</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss\ \U\T\C"/>
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd HH:mm:ss UTC"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -123,21 +67,13 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -175,7 +111,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -209,7 +145,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -244,10 +179,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -420,103 +354,284 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="6" max="6" width="20.7109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>season</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>species</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>tag</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>rings</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>crc</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>release_ts</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>catch_location</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
       <c r="A2">
         <v>2023</v>
       </c>
-      <c r="B2" t="s">
-        <v>7</v>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>redshank</t>
+        </is>
       </c>
       <c r="C2">
-        <v>3040</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
+        <v>3027</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>1598627</t>
+        </is>
       </c>
       <c r="F2" s="2">
-        <v>45185.041666666672</v>
-      </c>
-      <c r="G2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>45184.37847222222</v>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>griend</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
       <c r="A3">
         <v>2023</v>
       </c>
-      <c r="B3" t="s">
-        <v>10</v>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>red knot</t>
+        </is>
       </c>
       <c r="C3">
-        <v>3085</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" t="s">
-        <v>12</v>
+        <v>3038</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Z108940</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Y7PNGY</t>
+        </is>
       </c>
       <c r="F3" s="2">
-        <v>45185.833333333328</v>
-      </c>
-      <c r="G3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>45185.77083333333</v>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>griend</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
       <c r="A4">
         <v>2023</v>
       </c>
-      <c r="B4" t="s">
-        <v>10</v>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>bar-tailed godwit</t>
+        </is>
       </c>
       <c r="C4">
-        <v>3086</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" t="s">
-        <v>14</v>
+        <v>3063</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>1598632</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>N6NYRP</t>
+        </is>
       </c>
       <c r="F4" s="2">
-        <v>45185.833333333328</v>
-      </c>
-      <c r="G4" t="s">
-        <v>9</v>
+        <v>45185.52083333333</v>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>griend</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5">
+        <v>2023</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>curlew</t>
+        </is>
+      </c>
+      <c r="C5">
+        <v>3100</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>5517484</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Y-W[X59]</t>
+        </is>
+      </c>
+      <c r="F5" s="2">
+        <v>45157</v>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>griend</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6">
+        <v>2023</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>oystercatcher</t>
+        </is>
+      </c>
+      <c r="C6">
+        <v>3158</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>5544903</t>
+        </is>
+      </c>
+      <c r="F6" s="2">
+        <v>45159.22916666667</v>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>griend</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7">
+        <v>2023</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>turnstone</t>
+        </is>
+      </c>
+      <c r="C7">
+        <v>3188</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Z111576</t>
+        </is>
+      </c>
+      <c r="F7" s="2">
+        <v>45186.3125</v>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>griend</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8">
+        <v>2023</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>dunlin</t>
+        </is>
+      </c>
+      <c r="C8">
+        <v>3212</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>H401982</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Y1YPYR</t>
+        </is>
+      </c>
+      <c r="F8" s="2">
+        <v>45184.43055555555</v>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>griend</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9">
+        <v>2023</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>sanderling</t>
+        </is>
+      </c>
+      <c r="C9">
+        <v>3288</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>H401577</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Y2NYYG</t>
+        </is>
+      </c>
+      <c r="F9" s="2">
+        <v>45157.625</v>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>griend</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated example data (timezone and rm species column)
</commit_message>
<xml_diff>
--- a/inst/extdata/tags_watlas_subset.xlsx
+++ b/inst/extdata/tags_watlas_subset.xlsx
@@ -15,9 +15,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd HH:mm:ss UTC"/>
-  </numFmts>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -55,12 +52,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -360,9 +356,6 @@
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="6" max="6" width="20.7109375" style="2" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1">
       <c r="A1" s="1" t="inlineStr">
@@ -418,8 +411,10 @@
           <t>1598627</t>
         </is>
       </c>
-      <c r="F2" s="2">
-        <v>45184.37847222222</v>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>2023-09-15 11:05:00</t>
+        </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -449,8 +444,10 @@
           <t>Y7PNGY</t>
         </is>
       </c>
-      <c r="F3" s="2">
-        <v>45185.77083333333</v>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>2023-09-16 20:30:00</t>
+        </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
@@ -480,8 +477,10 @@
           <t>N6NYRP</t>
         </is>
       </c>
-      <c r="F4" s="2">
-        <v>45185.52083333333</v>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>2023-09-16 14:30:00</t>
+        </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
@@ -511,8 +510,10 @@
           <t>Y-W[X59]</t>
         </is>
       </c>
-      <c r="F5" s="2">
-        <v>45157</v>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>2023-08-19 02:00:00</t>
+        </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -537,8 +538,10 @@
           <t>5544903</t>
         </is>
       </c>
-      <c r="F6" s="2">
-        <v>45159.22916666667</v>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>2023-08-21 07:30:00</t>
+        </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
@@ -563,8 +566,10 @@
           <t>Z111576</t>
         </is>
       </c>
-      <c r="F7" s="2">
-        <v>45186.3125</v>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>2023-09-17 09:30:00</t>
+        </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
@@ -594,8 +599,10 @@
           <t>Y1YPYR</t>
         </is>
       </c>
-      <c r="F8" s="2">
-        <v>45184.43055555555</v>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>2023-09-15 12:20:00</t>
+        </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
@@ -625,8 +632,10 @@
           <t>Y2NYYG</t>
         </is>
       </c>
-      <c r="F9" s="2">
-        <v>45157.625</v>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>2023-08-19 17:00:00</t>
+        </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
changed speed filter to 35 m/s and season to year
</commit_message>
<xml_diff>
--- a/inst/extdata/tags_watlas_subset.xlsx
+++ b/inst/extdata/tags_watlas_subset.xlsx
@@ -1,21 +1,143 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkrietsch\GitHub_R_packages\tools4watlas\inst\extdata\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E065259B-9210-465E-97C0-3BA01AAF084E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="29970" yWindow="1170" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tags_watlas_all" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="37">
+  <si>
+    <t>species</t>
+  </si>
+  <si>
+    <t>tag</t>
+  </si>
+  <si>
+    <t>rings</t>
+  </si>
+  <si>
+    <t>crc</t>
+  </si>
+  <si>
+    <t>release_ts</t>
+  </si>
+  <si>
+    <t>catch_location</t>
+  </si>
+  <si>
+    <t>redshank</t>
+  </si>
+  <si>
+    <t>1598627</t>
+  </si>
+  <si>
+    <t>2023-09-15 11:05:00</t>
+  </si>
+  <si>
+    <t>griend</t>
+  </si>
+  <si>
+    <t>red knot</t>
+  </si>
+  <si>
+    <t>Z108940</t>
+  </si>
+  <si>
+    <t>Y7PNGY</t>
+  </si>
+  <si>
+    <t>2023-09-16 20:30:00</t>
+  </si>
+  <si>
+    <t>bar-tailed godwit</t>
+  </si>
+  <si>
+    <t>1598632</t>
+  </si>
+  <si>
+    <t>N6NYRP</t>
+  </si>
+  <si>
+    <t>2023-09-16 14:30:00</t>
+  </si>
+  <si>
+    <t>curlew</t>
+  </si>
+  <si>
+    <t>5517484</t>
+  </si>
+  <si>
+    <t>Y-W[X59]</t>
+  </si>
+  <si>
+    <t>2023-08-19 02:00:00</t>
+  </si>
+  <si>
+    <t>oystercatcher</t>
+  </si>
+  <si>
+    <t>5544903</t>
+  </si>
+  <si>
+    <t>2023-08-21 07:30:00</t>
+  </si>
+  <si>
+    <t>turnstone</t>
+  </si>
+  <si>
+    <t>Z111576</t>
+  </si>
+  <si>
+    <t>2023-09-17 09:30:00</t>
+  </si>
+  <si>
+    <t>dunlin</t>
+  </si>
+  <si>
+    <t>H401982</t>
+  </si>
+  <si>
+    <t>Y1YPYR</t>
+  </si>
+  <si>
+    <t>2023-09-15 12:20:00</t>
+  </si>
+  <si>
+    <t>sanderling</t>
+  </si>
+  <si>
+    <t>H401577</t>
+  </si>
+  <si>
+    <t>Y2NYYG</t>
+  </si>
+  <si>
+    <t>2023-08-19 17:00:00</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -63,13 +185,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -107,7 +237,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -141,6 +271,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -175,9 +306,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -350,297 +482,211 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>season</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>species</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>tag</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>rings</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>crc</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>release_ts</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>catch_location</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2023</v>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>redshank</t>
-        </is>
+      <c r="B2" t="s">
+        <v>6</v>
       </c>
       <c r="C2">
         <v>3027</v>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>1598627</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>2023-09-15 11:05:00</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>griend</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2023</v>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>red knot</t>
-        </is>
+      <c r="B3" t="s">
+        <v>10</v>
       </c>
       <c r="C3">
         <v>3038</v>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Z108940</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Y7PNGY</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>2023-09-16 20:30:00</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>griend</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2023</v>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>bar-tailed godwit</t>
-        </is>
+      <c r="B4" t="s">
+        <v>14</v>
       </c>
       <c r="C4">
         <v>3063</v>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>1598632</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>N6NYRP</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>2023-09-16 14:30:00</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>griend</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2023</v>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>curlew</t>
-        </is>
+      <c r="B5" t="s">
+        <v>18</v>
       </c>
       <c r="C5">
         <v>3100</v>
       </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>5517484</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Y-W[X59]</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>2023-08-19 02:00:00</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>griend</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
+      <c r="D5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2023</v>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>oystercatcher</t>
-        </is>
+      <c r="B6" t="s">
+        <v>22</v>
       </c>
       <c r="C6">
         <v>3158</v>
       </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>5544903</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>2023-08-21 07:30:00</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>griend</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
+      <c r="D6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2023</v>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>turnstone</t>
-        </is>
+      <c r="B7" t="s">
+        <v>25</v>
       </c>
       <c r="C7">
         <v>3188</v>
       </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>Z111576</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>2023-09-17 09:30:00</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>griend</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
+      <c r="D7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" t="s">
+        <v>27</v>
+      </c>
+      <c r="G7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2023</v>
       </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>dunlin</t>
-        </is>
+      <c r="B8" t="s">
+        <v>28</v>
       </c>
       <c r="C8">
         <v>3212</v>
       </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>H401982</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>Y1YPYR</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>2023-09-15 12:20:00</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>griend</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
+      <c r="D8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2023</v>
       </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>sanderling</t>
-        </is>
+      <c r="B9" t="s">
+        <v>32</v>
       </c>
       <c r="C9">
         <v>3288</v>
       </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>H401577</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>Y2NYYG</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>2023-08-19 17:00:00</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>griend</t>
-        </is>
+      <c r="D9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F9" t="s">
+        <v>35</v>
+      </c>
+      <c r="G9" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>